<commit_message>
finished markup rebuild using openpyxl.
</commit_message>
<xml_diff>
--- a/sample_data/SRO658Markup.xlsx
+++ b/sample_data/SRO658Markup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wv492f\Documents\Git\SRO658\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wv492f\Documents\VSCode_Projects\cross-checker\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E257179-04D0-4898-A10A-6D39D4676A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8BB4C8-D416-40A0-97C4-4CEBA5F2438E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39C8E638-C7C7-407E-B117-7F3298F6CE42}"/>
+    <workbookView xWindow="4740" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{39C8E638-C7C7-407E-B117-7F3298F6CE42}"/>
   </bookViews>
   <sheets>
     <sheet name="737MAX EDFCS Requirements_Valid" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Object Identifier</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Verification: -10 Requirement Verification Close-Out</t>
-  </si>
-  <si>
-    <t>EDFCS2630</t>
   </si>
   <si>
     <t>3.2.5.2.24</t>
@@ -899,7 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -915,6 +912,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1297,9 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B43566A-DCD0-426B-BE22-7F550EE06EFA}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1353,7 @@
   <sheetData>
     <row r="1" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1493,118 +1493,115 @@
     </row>
     <row r="2" spans="1:46" s="3" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AH2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AM2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>